<commit_message>
modif navbar avec ajout d'un dropdown
</commit_message>
<xml_diff>
--- a/images produits + descriptions.xlsx
+++ b/images produits + descriptions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SymfonyProjects\e-commerce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{132FFA19-0A61-454A-BC88-0C554BF76BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08641B1B-FD38-47B4-AEB4-4EB9225A1001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2A41480D-03EE-4DC5-AACB-80600BF1585E}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>CANOE KAYAK GONFLABLE RANDONNEE FOND HAUTE PRESSION DROP STITCH X100+ 2 PLACES</t>
   </si>
@@ -138,13 +137,49 @@
   </si>
   <si>
     <t>Nos concepteurs campeurs ont conçu ce matelas autogonflant Ultim Comfort très épais pour un campeur cherchant le confort comme à la maison. Notre motivation ? Vous proposer un matelas de 70 cm autogonflant très épais, jumelable et très simple d'installation pour un confort comme à la maison en camping.</t>
+  </si>
+  <si>
+    <t>LUNETTES DE SOLEIL RANDONNÉE - MH140 - ADULTE - POLARISANTES CATÉGORIE 3</t>
+  </si>
+  <si>
+    <t>C:\SymfonyProjects\e-commerce\public\pictures\lunettes-de-soleil-randonnee-mh140-adulte-polarisantes-categorie-3.avif</t>
+  </si>
+  <si>
+    <t>Nos ingénieurs optiques ont développé ces lunettes de soleil pour la randonnée. Idéales pour un usage occasionnel en montagne grâce à leur légèreté. Les verres anti-UV bloquent 100% des rayons nocifs et la catégorie 3 vous protège de l’éblouissement. La technologie des verres polarisants vous permet de mieux distinguer les reliefs et contrastes.</t>
+  </si>
+  <si>
+    <t>CHAUSSETTES DE RUNNING RUN100 NOIRE X3</t>
+  </si>
+  <si>
+    <t>C:\SymfonyProjects\e-commerce\public\pictures\chaussettes-de-running-run100-noire-x3.avif</t>
+  </si>
+  <si>
+    <t>Nos équipes de conception ont développé ces chaussettes de running pour que votre pied soit protégé des risques d'ampoules lors de vos sorties de course à pied. Des chaussettes de running à petit prix ? Grâce à leur fil en coton, leur tricotage fin et aéré, elles sont idéales pour la course à pied à petit budget.</t>
+  </si>
+  <si>
+    <t>MONTRE CARDIO GPS GARMIN FORERUNNER 245 GRISE</t>
+  </si>
+  <si>
+    <t>C:\SymfonyProjects\e-commerce\public\pictures\montre-cardio-gps-garmin-forerunner-245-grise.avif</t>
+  </si>
+  <si>
+    <t>Conçue pour les runners, coureurs de 10km, de semi et de marathon. Elle suit vos statistiques, traite les données et acquiert toutes les informations sur vos performances, votre technique de course, l'historique de vos entraînements et même vos objectifs.</t>
+  </si>
+  <si>
+    <t>C:\SymfonyProjects\e-commerce\public\pictures\sac-a-dos-de-randonnee-30l-nh-arpenaz-500.avif</t>
+  </si>
+  <si>
+    <t>SAC À DOS DE RANDONNÉE 30L - NH ARPENAZ 500</t>
+  </si>
+  <si>
+    <t>Nos concepteurs randonneurs ont conçu ce sac à dos NH Arpenaz 500 30 litres pour accompagner vos randonnées à la journée en plaine, forêt ou sur le littoral. Notre motivation ? Vous proposer un sac à dos confortable et très accessoirisé pour profiter de vos randonnées ! Retrouvez une poche pour conserver au frais votre pique-nique et une poche téléphone.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -501,20 +536,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5B4725-0856-4A67-A319-B8AC47011291}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="66.140625" customWidth="1"/>
-    <col min="2" max="2" width="92.140625" customWidth="1"/>
-    <col min="3" max="3" width="158.28515625" customWidth="1"/>
+    <col min="1" max="1" width="66.109375" customWidth="1"/>
+    <col min="2" max="2" width="163.21875" customWidth="1"/>
+    <col min="3" max="3" width="158.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -525,7 +560,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -536,7 +571,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -547,7 +582,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -558,7 +593,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -569,7 +604,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30">
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -580,7 +615,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -591,12 +626,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -607,7 +642,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -618,7 +653,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -629,7 +664,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -640,24 +675,58 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>34</v>
+      </c>
       <c r="B16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>